<commit_message>
Minor configurations to adapt to kong
</commit_message>
<xml_diff>
--- a/backend/API Calls.xlsx
+++ b/backend/API Calls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\study_buddy\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03518523-5C3E-4E85-A50E-D009415784FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171EBFF7-84C6-4D21-A429-74CAC866A15B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C18B1A27-F6D6-4125-8D92-62D274593774}"/>
   </bookViews>
@@ -252,64 +252,14 @@
 update_status</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>get_all</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">find_by_username
+    <t>get_all
+find_by_username
 find_by_user_id
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>create_user
+create_user
 delete_user</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">get_all_payment
+  </si>
+  <si>
+    <t>get_all_payment
 get_payment_status
 get_payout_status
 find_by_payment_id
@@ -320,19 +270,8 @@
 update_status_by_liaise_id
 delete_payment
 create_checkout_session
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>order_success
+order_success
 order_failure</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -376,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -389,9 +328,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -713,7 +649,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,10 +699,10 @@
       <c r="B2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -778,10 +714,10 @@
       <c r="G2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>